<commit_message>
Posting my diagnosis rates post
</commit_message>
<xml_diff>
--- a/assets/Dx stats.xlsx
+++ b/assets/Dx stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\atelfo.github.io\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCD29C2-362C-4CC2-AC49-E045BE0ACC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D822BF-D3E6-4D9F-B585-AAF29000DCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{81DE6EE8-0027-492D-AF58-69F03109B8D0}"/>
+    <workbookView xWindow="-28920" yWindow="2280" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{81DE6EE8-0027-492D-AF58-69F03109B8D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Average time to Dx" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="413">
   <si>
     <t>Indication</t>
   </si>
@@ -1269,14 +1269,24 @@
   </si>
   <si>
     <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>M (per year)</t>
+  </si>
+  <si>
+    <t>in months</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1372,7 +1382,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1386,6 +1396,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1531,6 +1542,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF5F5F5"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2409,6 +2425,187 @@
           <c:h val="0.82078458491733819"/>
         </c:manualLayout>
       </c:layout>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Time to Dx vs. mortality'!$AC$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>p(Dx+)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F5F5F5"/>
+            </a:solidFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Time to Dx vs. mortality'!$AH$3:$AH$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.6000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Time to Dx vs. mortality'!$AF$3:$AF$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000%</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99997343860111243</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65132155989999985</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.40950999999999982</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23156652857908377</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16104722339245814</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12339662821723285</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9999999999999978E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.7830248213842315E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.1316701949486232E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4510615394370281E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5996253574703254E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.0851637639023202E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7406806147310161E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4938794558884472E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.3083718633998487E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1638466884251741E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0480741793785553E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.5325035687154891E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.7416109546967213E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-75BA-4D9D-A7B6-FC7E1CC8EE17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="614854224"/>
+        <c:axId val="614851272"/>
+      </c:areaChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -2454,7 +2651,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7DD25DC3-AD51-4E42-9D2D-DA25FAB2B653}" type="CELLRANGE">
+                    <a:fld id="{6C4B76A4-C4EC-4DB9-9E23-139D5FFF84BB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2804,60 +3001,18 @@
               <c:idx val="33"/>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+                  <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:pPr algn="l">
-                      <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="AkzidenzGrotesk" panose="02000503050000020003" pitchFamily="2" charset="0"/>
-                        <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:fld id="{EA532417-C7E4-40A5-8CEB-EF2EE90E8490}" type="CELLRANGE">
+                    <a:fld id="{10F8B474-8EA2-4BEF-9016-355EBF8C2EE9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
-                      <a:pPr algn="l">
-                        <a:defRPr/>
-                      </a:pPr>
+                      <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr algn="l">
-                    <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="AkzidenzGrotesk" panose="02000503050000020003" pitchFamily="2" charset="0"/>
-                      <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2882,13 +3037,19 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="34"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.9391293020964542E-3"/>
+                  <c:y val="-2.1583562996657559E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D3F9FAE-9D8F-45B8-BD7B-80E60CB670B3}" type="CELLRANGE">
-                      <a:rPr lang="en-GB"/>
+                    <a:fld id="{EA9C7542-62B0-4A54-9307-DDB32433361F}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -2905,7 +3066,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2976,7 +3136,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{25E39B18-1ACC-4ACB-9943-69B95AA91166}" type="CELLRANGE">
+                    <a:fld id="{ABF079DE-47C0-4955-9D52-D4E9B113BFE7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3019,9 +3179,32 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="42"/>
-              <c:delete val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{585B8082-DE19-434A-A4B7-1280CD2B5F46}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000002C-0F27-4D3C-B3C1-6C30F6F61EF9}"/>
                 </c:ext>
@@ -3029,9 +3212,32 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="43"/>
-              <c:delete val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1CD00530-0906-4C8C-9005-7D7C8D80B917}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-GB"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000002D-0F27-4D3C-B3C1-6C30F6F61EF9}"/>
                 </c:ext>
@@ -3044,7 +3250,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E66407D-F620-4B97-B7E5-51D348E4EE4E}" type="CELLRANGE">
+                    <a:fld id="{F4326E70-2503-425A-A902-36C3CCBA0EA8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3082,7 +3288,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFE02A94-1107-4FD9-9286-27393608F70A}" type="CELLRANGE">
+                    <a:fld id="{FB1CCE45-66C6-4963-9899-A4FAB6494AC6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3126,7 +3332,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7DEBF887-F47F-403F-842D-D5D0E758F9E8}" type="CELLRANGE">
+                    <a:fld id="{DF531A20-A14E-4A6D-9382-B203DBF5B91F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3174,7 +3380,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8796E5A8-E471-478A-A81C-9FA018EF2462}" type="CELLRANGE">
+                    <a:fld id="{3ED5CE5B-6FEB-4570-918D-290275205B5D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3207,7 +3413,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48662B66-C5BE-4398-A422-88F880661D42}" type="CELLRANGE">
+                    <a:fld id="{D1727B3A-8AF6-45F3-A4F2-CF7A64A7211F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3240,7 +3446,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D8205B1-9130-44B9-9E2D-DA70747596D3}" type="CELLRANGE">
+                    <a:fld id="{7E945B53-F389-4020-AA93-AA7C56626472}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3273,7 +3479,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9114D1E-83C3-49CA-B468-C40215B3FF33}" type="CELLRANGE">
+                    <a:fld id="{D0561D9B-8EFC-4B9D-89B8-A2F7D7EF7263}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3363,7 +3569,21 @@
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showDataLabelsRange val="1"/>
-                <c15:showLeaderLines val="0"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -3883,8 +4103,6 @@
         <c:axId val="701756640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="150"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4090,6 +4308,39 @@
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="614851272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.8"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.0000%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="614854224"/>
+        <c:crossesAt val="21"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:dateAx>
+        <c:axId val="614854224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="614851272"/>
+        <c:crosses val="max"/>
+        <c:auto val="0"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -5256,16 +5507,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>434209</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>108059</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>316978</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>42117</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>120214</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>184259</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>2983</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>118317</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5292,16 +5543,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>575701</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>172570</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>199830</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>113954</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>582705</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>206834</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>109472</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5328,16 +5579,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>145676</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>58615</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>386523</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>186523</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>446942</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>58615</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>566057</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>186523</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5352,8 +5603,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14396541" y="9964615"/>
-          <a:ext cx="6990747" cy="0"/>
+          <a:off x="16742309" y="9330523"/>
+          <a:ext cx="8104334" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -5458,7 +5709,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9434C479-1C7F-4F7F-A60F-07D41922F376}" name="Table36" displayName="Table36" ref="A1:F3" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9434C479-1C7F-4F7F-A60F-07D41922F376}" name="Table36" displayName="Table36" ref="A1:F3" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:F3" xr:uid="{9434C479-1C7F-4F7F-A60F-07D41922F376}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9E5052FC-8865-4C45-ACF9-01CED35EEDD1}" name="Indication"/>
@@ -5473,7 +5724,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{85050C1A-9E69-474A-800C-037D14C54F8E}" name="Table35" displayName="Table35" ref="A1:F16" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{85050C1A-9E69-474A-800C-037D14C54F8E}" name="Table35" displayName="Table35" ref="A1:F16" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:F16" xr:uid="{0CD6A652-9B8C-4BE6-A3C4-3A018D44C79C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B3D76C6A-4FD0-410E-8704-B1649668327E}" name="Indication"/>
@@ -5786,8 +6037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA5513E-26DC-4C85-8B8F-1046086877AA}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I69" sqref="I33:I69"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5866,7 +6117,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="3">
-        <f>IF(G2="Days", E2/30, IF(G2="Years", E2*12, IF(G2="Weeks", E2/4, E2)))</f>
+        <f t="shared" ref="I2:I33" si="0">IF(G2="Days", E2/30, IF(G2="Years", E2*12, IF(G2="Weeks", E2/4, E2)))</f>
         <v>2.222222222222222E-2</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -5900,7 +6151,7 @@
         <v>16</v>
       </c>
       <c r="I3" s="3">
-        <f>IF(G3="Days", E3/30, IF(G3="Years", E3*12, IF(G3="Weeks", E3/4, E3)))</f>
+        <f t="shared" si="0"/>
         <v>0.23333333333333334</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -5934,7 +6185,7 @@
         <v>16</v>
       </c>
       <c r="I4" s="3">
-        <f>IF(G4="Days", E4/30, IF(G4="Years", E4*12, IF(G4="Weeks", E4/4, E4)))</f>
+        <f t="shared" si="0"/>
         <v>0.25666666666666665</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -5969,7 +6220,7 @@
         <v>16</v>
       </c>
       <c r="I5" s="3">
-        <f>IF(G5="Days", E5/30, IF(G5="Years", E5*12, IF(G5="Weeks", E5/4, E5)))</f>
+        <f t="shared" si="0"/>
         <v>0.31</v>
       </c>
       <c r="J5" t="s">
@@ -6003,7 +6254,7 @@
         <v>16</v>
       </c>
       <c r="I6" s="3">
-        <f>IF(G6="Days", E6/30, IF(G6="Years", E6*12, IF(G6="Weeks", E6/4, E6)))</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -6040,7 +6291,7 @@
         <v>233</v>
       </c>
       <c r="I7" s="3">
-        <f>IF(G7="Days", E7/30, IF(G7="Years", E7*12, IF(G7="Weeks", E7/4, E7)))</f>
+        <f t="shared" si="0"/>
         <v>1.325</v>
       </c>
       <c r="J7" t="s">
@@ -6077,7 +6328,7 @@
         <v>215</v>
       </c>
       <c r="I8" s="3">
-        <f>IF(G8="Days", E8/30, IF(G8="Years", E8*12, IF(G8="Weeks", E8/4, E8)))</f>
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
       <c r="J8" s="2" t="s">
@@ -6114,7 +6365,7 @@
         <v>110</v>
       </c>
       <c r="I9" s="3">
-        <f>IF(G9="Days", E9/30, IF(G9="Years", E9*12, IF(G9="Weeks", E9/4, E9)))</f>
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
       <c r="J9" t="s">
@@ -6151,7 +6402,7 @@
         <v>272</v>
       </c>
       <c r="I10" s="3">
-        <f>IF(G10="Days", E10/30, IF(G10="Years", E10*12, IF(G10="Weeks", E10/4, E10)))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -6185,7 +6436,7 @@
         <v>16</v>
       </c>
       <c r="I11" s="3">
-        <f>IF(G11="Days", E11/30, IF(G11="Years", E11*12, IF(G11="Weeks", E11/4, E11)))</f>
+        <f t="shared" si="0"/>
         <v>2.14</v>
       </c>
       <c r="J11" s="2" t="s">
@@ -6222,7 +6473,7 @@
         <v>117</v>
       </c>
       <c r="I12" s="3">
-        <f>IF(G12="Days", E12/30, IF(G12="Years", E12*12, IF(G12="Weeks", E12/4, E12)))</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -6259,7 +6510,7 @@
         <v>188</v>
       </c>
       <c r="I13" s="3">
-        <f>IF(G13="Days", E13/30, IF(G13="Years", E13*12, IF(G13="Weeks", E13/4, E13)))</f>
+        <f t="shared" si="0"/>
         <v>2.4666666666666668</v>
       </c>
       <c r="J13" s="2" t="s">
@@ -6296,7 +6547,7 @@
         <v>208</v>
       </c>
       <c r="I14" s="3">
-        <f>IF(G14="Days", E14/30, IF(G14="Years", E14*12, IF(G14="Weeks", E14/4, E14)))</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="J14" s="2" t="s">
@@ -6330,7 +6581,7 @@
         <v>31</v>
       </c>
       <c r="I15" s="3">
-        <f>IF(G15="Days", E15/30, IF(G15="Years", E15*12, IF(G15="Weeks", E15/4, E15)))</f>
+        <f t="shared" si="0"/>
         <v>2.8666666666666667</v>
       </c>
       <c r="J15" t="s">
@@ -6367,7 +6618,7 @@
         <v>160</v>
       </c>
       <c r="I16" s="3">
-        <f>IF(G16="Days", E16/30, IF(G16="Years", E16*12, IF(G16="Weeks", E16/4, E16)))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J16" s="2" t="s">
@@ -6401,7 +6652,7 @@
         <v>16</v>
       </c>
       <c r="I17" s="3">
-        <f>IF(G17="Days", E17/30, IF(G17="Years", E17*12, IF(G17="Weeks", E17/4, E17)))</f>
+        <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
       <c r="J17" s="2" t="s">
@@ -6435,7 +6686,7 @@
         <v>27</v>
       </c>
       <c r="I18" s="3">
-        <f>IF(G18="Days", E18/30, IF(G18="Years", E18*12, IF(G18="Weeks", E18/4, E18)))</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="J18" s="2" t="s">
@@ -6469,7 +6720,7 @@
         <v>27</v>
       </c>
       <c r="I19" s="3">
-        <f>IF(G19="Days", E19/30, IF(G19="Years", E19*12, IF(G19="Weeks", E19/4, E19)))</f>
+        <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
       <c r="J19" t="s">
@@ -6503,7 +6754,7 @@
         <v>13</v>
       </c>
       <c r="I20" s="3">
-        <f>IF(G20="Days", E20/30, IF(G20="Years", E20*12, IF(G20="Weeks", E20/4, E20)))</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J20" s="2" t="s">
@@ -6540,7 +6791,7 @@
         <v>259</v>
       </c>
       <c r="I21" s="3">
-        <f>IF(G21="Days", E21/30, IF(G21="Years", E21*12, IF(G21="Weeks", E21/4, E21)))</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J21" s="2" t="s">
@@ -6574,7 +6825,7 @@
         <v>16</v>
       </c>
       <c r="I22" s="3">
-        <f>IF(G22="Days", E22/30, IF(G22="Years", E22*12, IF(G22="Weeks", E22/4, E22)))</f>
+        <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
       <c r="J22" s="2" t="s">
@@ -6608,7 +6859,7 @@
         <v>27</v>
       </c>
       <c r="I23" s="3">
-        <f>IF(G23="Days", E23/30, IF(G23="Years", E23*12, IF(G23="Weeks", E23/4, E23)))</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="J23" s="2" t="s">
@@ -6642,7 +6893,7 @@
         <v>16</v>
       </c>
       <c r="I24" s="3">
-        <f>IF(G24="Days", E24/30, IF(G24="Years", E24*12, IF(G24="Weeks", E24/4, E24)))</f>
+        <f t="shared" si="0"/>
         <v>5.0666666666666664</v>
       </c>
       <c r="J24" t="s">
@@ -6676,7 +6927,7 @@
         <v>27</v>
       </c>
       <c r="I25" s="3">
-        <f>IF(G25="Days", E25/30, IF(G25="Years", E25*12, IF(G25="Weeks", E25/4, E25)))</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J25" s="2" t="s">
@@ -6713,7 +6964,7 @@
         <v>158</v>
       </c>
       <c r="I26" s="3">
-        <f>IF(G26="Days", E26/30, IF(G26="Years", E26*12, IF(G26="Weeks", E26/4, E26)))</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J26" s="2" t="s">
@@ -6747,7 +6998,7 @@
         <v>27</v>
       </c>
       <c r="I27" s="3">
-        <f>IF(G27="Days", E27/30, IF(G27="Years", E27*12, IF(G27="Weeks", E27/4, E27)))</f>
+        <f t="shared" si="0"/>
         <v>6.1</v>
       </c>
       <c r="J27" s="2" t="s">
@@ -6784,7 +7035,7 @@
         <v>191</v>
       </c>
       <c r="I28" s="3">
-        <f>IF(G28="Days", E28/30, IF(G28="Years", E28*12, IF(G28="Weeks", E28/4, E28)))</f>
+        <f t="shared" si="0"/>
         <v>6.19</v>
       </c>
       <c r="J28" t="s">
@@ -6821,7 +7072,7 @@
         <v>170</v>
       </c>
       <c r="I29" s="3">
-        <f>IF(G29="Days", E29/30, IF(G29="Years", E29*12, IF(G29="Weeks", E29/4, E29)))</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="J29" s="2" t="s">
@@ -6858,7 +7109,7 @@
         <v>179</v>
       </c>
       <c r="I30" s="3">
-        <f>IF(G30="Days", E30/30, IF(G30="Years", E30*12, IF(G30="Weeks", E30/4, E30)))</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="J30" t="s">
@@ -6895,7 +7146,7 @@
         <v>277</v>
       </c>
       <c r="I31" s="3">
-        <f>IF(G31="Days", E31/30, IF(G31="Years", E31*12, IF(G31="Weeks", E31/4, E31)))</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="J31" s="2" t="s">
@@ -6932,7 +7183,7 @@
         <v>63</v>
       </c>
       <c r="I32" s="3">
-        <f>IF(G32="Days", E32/30, IF(G32="Years", E32*12, IF(G32="Weeks", E32/4, E32)))</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="J32" t="s">
@@ -6969,7 +7220,7 @@
         <v>108</v>
       </c>
       <c r="I33" s="3">
-        <f>IF(G33="Days", E33/30, IF(G33="Years", E33*12, IF(G33="Weeks", E33/4, E33)))</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="J33" s="2" t="s">
@@ -7006,7 +7257,7 @@
         <v>165</v>
       </c>
       <c r="I34" s="3">
-        <f>IF(G34="Days", E34/30, IF(G34="Years", E34*12, IF(G34="Weeks", E34/4, E34)))</f>
+        <f t="shared" ref="I34:I65" si="1">IF(G34="Days", E34/30, IF(G34="Years", E34*12, IF(G34="Weeks", E34/4, E34)))</f>
         <v>12</v>
       </c>
       <c r="J34" s="2" t="s">
@@ -7040,7 +7291,7 @@
         <v>27</v>
       </c>
       <c r="I35" s="3">
-        <f>IF(G35="Days", E35/30, IF(G35="Years", E35*12, IF(G35="Weeks", E35/4, E35)))</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="J35" s="2" t="s">
@@ -7077,7 +7328,7 @@
         <v>93</v>
       </c>
       <c r="I36" s="3">
-        <f>IF(G36="Days", E36/30, IF(G36="Years", E36*12, IF(G36="Weeks", E36/4, E36)))</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="J36" s="2" t="s">
@@ -7114,7 +7365,7 @@
         <v>298</v>
       </c>
       <c r="I37" s="3">
-        <f>IF(G37="Days", E37/30, IF(G37="Years", E37*12, IF(G37="Weeks", E37/4, E37)))</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="J37" s="2" t="s">
@@ -7148,7 +7399,7 @@
         <v>27</v>
       </c>
       <c r="I38" s="3">
-        <f>IF(G38="Days", E38/30, IF(G38="Years", E38*12, IF(G38="Weeks", E38/4, E38)))</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="J38" s="2" t="s">
@@ -7182,7 +7433,7 @@
         <v>27</v>
       </c>
       <c r="I39" s="3">
-        <f>IF(G39="Days", E39/30, IF(G39="Years", E39*12, IF(G39="Weeks", E39/4, E39)))</f>
+        <f t="shared" si="1"/>
         <v>14.3</v>
       </c>
       <c r="J39" t="s">
@@ -7219,7 +7470,7 @@
         <v>138</v>
       </c>
       <c r="I40" s="3">
-        <f>IF(G40="Days", E40/30, IF(G40="Years", E40*12, IF(G40="Weeks", E40/4, E40)))</f>
+        <f t="shared" si="1"/>
         <v>14.399999999999999</v>
       </c>
       <c r="J40" s="2" t="s">
@@ -7253,7 +7504,7 @@
         <v>27</v>
       </c>
       <c r="I41" s="3">
-        <f>IF(G41="Days", E41/30, IF(G41="Years", E41*12, IF(G41="Weeks", E41/4, E41)))</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="J41" t="s">
@@ -7290,7 +7541,7 @@
         <v>57</v>
       </c>
       <c r="I42" s="3">
-        <f>IF(G42="Days", E42/30, IF(G42="Years", E42*12, IF(G42="Weeks", E42/4, E42)))</f>
+        <f t="shared" si="1"/>
         <v>18.5</v>
       </c>
       <c r="J42" s="2" t="s">
@@ -7327,7 +7578,7 @@
         <v>292</v>
       </c>
       <c r="I43" s="3">
-        <f>IF(G43="Days", E43/30, IF(G43="Years", E43*12, IF(G43="Weeks", E43/4, E43)))</f>
+        <f t="shared" si="1"/>
         <v>19.200000000000003</v>
       </c>
       <c r="J43" s="2" t="s">
@@ -7358,7 +7609,7 @@
         <v>27</v>
       </c>
       <c r="I44" s="3">
-        <f>IF(G44="Days", E44/30, IF(G44="Years", E44*12, IF(G44="Weeks", E44/4, E44)))</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="J44" s="2" t="s">
@@ -7395,7 +7646,7 @@
         <v>151</v>
       </c>
       <c r="I45" s="3">
-        <f>IF(G45="Days", E45/30, IF(G45="Years", E45*12, IF(G45="Weeks", E45/4, E45)))</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="J45" s="2" t="s">
@@ -7432,7 +7683,7 @@
         <v>196</v>
       </c>
       <c r="I46" s="3">
-        <f>IF(G46="Days", E46/30, IF(G46="Years", E46*12, IF(G46="Weeks", E46/4, E46)))</f>
+        <f t="shared" si="1"/>
         <v>21.3</v>
       </c>
       <c r="J46" s="2" t="s">
@@ -7466,7 +7717,7 @@
         <v>27</v>
       </c>
       <c r="I47" s="3">
-        <f>IF(G47="Days", E47/30, IF(G47="Years", E47*12, IF(G47="Weeks", E47/4, E47)))</f>
+        <f t="shared" si="1"/>
         <v>22.6</v>
       </c>
       <c r="J47" s="2" t="s">
@@ -7503,7 +7754,7 @@
         <v>265</v>
       </c>
       <c r="I48" s="3">
-        <f>IF(G48="Days", E48/30, IF(G48="Years", E48*12, IF(G48="Weeks", E48/4, E48)))</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="J48" t="s">
@@ -7540,7 +7791,7 @@
         <v>45</v>
       </c>
       <c r="I49" s="3">
-        <f>IF(G49="Days", E49/30, IF(G49="Years", E49*12, IF(G49="Weeks", E49/4, E49)))</f>
+        <f t="shared" si="1"/>
         <v>25.200000000000003</v>
       </c>
       <c r="J49" t="s">
@@ -7577,7 +7828,7 @@
         <v>98</v>
       </c>
       <c r="I50" s="3">
-        <f>IF(G50="Days", E50/30, IF(G50="Years", E50*12, IF(G50="Weeks", E50/4, E50)))</f>
+        <f t="shared" si="1"/>
         <v>25.200000000000003</v>
       </c>
       <c r="J50" t="s">
@@ -7614,7 +7865,7 @@
         <v>46</v>
       </c>
       <c r="I51" s="3">
-        <f>IF(G51="Days", E51/30, IF(G51="Years", E51*12, IF(G51="Weeks", E51/4, E51)))</f>
+        <f t="shared" si="1"/>
         <v>26.400000000000002</v>
       </c>
       <c r="J51" t="s">
@@ -7651,7 +7902,7 @@
         <v>182</v>
       </c>
       <c r="I52" s="3">
-        <f>IF(G52="Days", E52/30, IF(G52="Years", E52*12, IF(G52="Weeks", E52/4, E52)))</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="J52" t="s">
@@ -7688,7 +7939,7 @@
         <v>252</v>
       </c>
       <c r="I53" s="3">
-        <f>IF(G53="Days", E53/30, IF(G53="Years", E53*12, IF(G53="Weeks", E53/4, E53)))</f>
+        <f t="shared" si="1"/>
         <v>28.75</v>
       </c>
       <c r="J53" s="2" t="s">
@@ -7722,7 +7973,7 @@
         <v>27</v>
       </c>
       <c r="I54" s="3">
-        <f>IF(G54="Days", E54/30, IF(G54="Years", E54*12, IF(G54="Weeks", E54/4, E54)))</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="J54" s="2" t="s">
@@ -7756,7 +8007,7 @@
         <v>27</v>
       </c>
       <c r="I55" s="3">
-        <f>IF(G55="Days", E55/30, IF(G55="Years", E55*12, IF(G55="Weeks", E55/4, E55)))</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="J55" t="s">
@@ -7793,7 +8044,7 @@
         <v>76</v>
       </c>
       <c r="I56" s="3">
-        <f>IF(G56="Days", E56/30, IF(G56="Years", E56*12, IF(G56="Weeks", E56/4, E56)))</f>
+        <f t="shared" si="1"/>
         <v>31.200000000000003</v>
       </c>
       <c r="J56" t="s">
@@ -7827,7 +8078,7 @@
         <v>27</v>
       </c>
       <c r="I57" s="3">
-        <f>IF(G57="Days", E57/30, IF(G57="Years", E57*12, IF(G57="Weeks", E57/4, E57)))</f>
+        <f t="shared" si="1"/>
         <v>32.89</v>
       </c>
       <c r="J57" s="2" t="s">
@@ -7864,7 +8115,7 @@
         <v>184</v>
       </c>
       <c r="I58" s="3">
-        <f>IF(G58="Days", E58/30, IF(G58="Years", E58*12, IF(G58="Weeks", E58/4, E58)))</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="J58" s="2" t="s">
@@ -7901,7 +8152,7 @@
         <v>36</v>
       </c>
       <c r="I59" s="3">
-        <f>IF(G59="Days", E59/30, IF(G59="Years", E59*12, IF(G59="Weeks", E59/4, E59)))</f>
+        <f t="shared" si="1"/>
         <v>33.599999999999994</v>
       </c>
       <c r="J59" t="s">
@@ -7935,7 +8186,7 @@
         <v>27</v>
       </c>
       <c r="I60" s="3">
-        <f>IF(G60="Days", E60/30, IF(G60="Years", E60*12, IF(G60="Weeks", E60/4, E60)))</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="J60" s="2" t="s">
@@ -7972,7 +8223,7 @@
         <v>44</v>
       </c>
       <c r="I61" s="3">
-        <f>IF(G61="Days", E61/30, IF(G61="Years", E61*12, IF(G61="Weeks", E61/4, E61)))</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="J61" t="s">
@@ -8009,7 +8260,7 @@
         <v>133</v>
       </c>
       <c r="I62" s="3">
-        <f>IF(G62="Days", E62/30, IF(G62="Years", E62*12, IF(G62="Weeks", E62/4, E62)))</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="J62" t="s">
@@ -8046,7 +8297,7 @@
         <v>53</v>
       </c>
       <c r="I63" s="3">
-        <f>IF(G63="Days", E63/30, IF(G63="Years", E63*12, IF(G63="Weeks", E63/4, E63)))</f>
+        <f t="shared" si="1"/>
         <v>37.200000000000003</v>
       </c>
       <c r="J63" t="s">
@@ -8080,7 +8331,7 @@
         <v>27</v>
       </c>
       <c r="I64" s="3">
-        <f>IF(G64="Days", E64/30, IF(G64="Years", E64*12, IF(G64="Weeks", E64/4, E64)))</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="J64" s="2" t="s">
@@ -8114,7 +8365,7 @@
         <v>27</v>
       </c>
       <c r="I65" s="3">
-        <f>IF(G65="Days", E65/30, IF(G65="Years", E65*12, IF(G65="Weeks", E65/4, E65)))</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J65" t="s">
@@ -8148,7 +8399,7 @@
         <v>33</v>
       </c>
       <c r="I66" s="3">
-        <f>IF(G66="Days", E66/30, IF(G66="Years", E66*12, IF(G66="Weeks", E66/4, E66)))</f>
+        <f t="shared" ref="I66:I95" si="2">IF(G66="Days", E66/30, IF(G66="Years", E66*12, IF(G66="Weeks", E66/4, E66)))</f>
         <v>43.2</v>
       </c>
       <c r="J66" s="2" t="s">
@@ -8185,7 +8436,7 @@
         <v>40</v>
       </c>
       <c r="I67" s="3">
-        <f>IF(G67="Days", E67/30, IF(G67="Years", E67*12, IF(G67="Weeks", E67/4, E67)))</f>
+        <f t="shared" si="2"/>
         <v>43.2</v>
       </c>
       <c r="J67" t="s">
@@ -8219,7 +8470,7 @@
         <v>27</v>
       </c>
       <c r="I68" s="3">
-        <f>IF(G68="Days", E68/30, IF(G68="Years", E68*12, IF(G68="Weeks", E68/4, E68)))</f>
+        <f t="shared" si="2"/>
         <v>43.6</v>
       </c>
       <c r="J68" t="s">
@@ -8253,7 +8504,7 @@
         <v>27</v>
       </c>
       <c r="I69" s="3">
-        <f>IF(G69="Days", E69/30, IF(G69="Years", E69*12, IF(G69="Weeks", E69/4, E69)))</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="J69" t="s">
@@ -8290,7 +8541,7 @@
         <v>51</v>
       </c>
       <c r="I70" s="3">
-        <f>IF(G70="Days", E70/30, IF(G70="Years", E70*12, IF(G70="Weeks", E70/4, E70)))</f>
+        <f t="shared" si="2"/>
         <v>45.599999999999994</v>
       </c>
       <c r="J70" t="s">
@@ -8327,7 +8578,7 @@
         <v>40</v>
       </c>
       <c r="I71" s="3">
-        <f>IF(G71="Days", E71/30, IF(G71="Years", E71*12, IF(G71="Weeks", E71/4, E71)))</f>
+        <f t="shared" si="2"/>
         <v>46.8</v>
       </c>
       <c r="J71" t="s">
@@ -8364,7 +8615,7 @@
         <v>37</v>
       </c>
       <c r="I72" s="3">
-        <f>IF(G72="Days", E72/30, IF(G72="Years", E72*12, IF(G72="Weeks", E72/4, E72)))</f>
+        <f t="shared" si="2"/>
         <v>50.400000000000006</v>
       </c>
       <c r="J72" t="s">
@@ -8401,7 +8652,7 @@
         <v>35</v>
       </c>
       <c r="I73" s="3">
-        <f>IF(G73="Days", E73/30, IF(G73="Years", E73*12, IF(G73="Weeks", E73/4, E73)))</f>
+        <f t="shared" si="2"/>
         <v>52.800000000000004</v>
       </c>
       <c r="J73" t="s">
@@ -8438,7 +8689,7 @@
         <v>68</v>
       </c>
       <c r="I74" s="3">
-        <f>IF(G74="Days", E74/30, IF(G74="Years", E74*12, IF(G74="Weeks", E74/4, E74)))</f>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="J74" t="s">
@@ -8475,7 +8726,7 @@
         <v>261</v>
       </c>
       <c r="I75" s="3">
-        <f>IF(G75="Days", E75/30, IF(G75="Years", E75*12, IF(G75="Weeks", E75/4, E75)))</f>
+        <f t="shared" si="2"/>
         <v>67.199999999999989</v>
       </c>
       <c r="J75" s="2" t="s">
@@ -8512,7 +8763,7 @@
         <v>217</v>
       </c>
       <c r="I76" s="3">
-        <f>IF(G76="Days", E76/30, IF(G76="Years", E76*12, IF(G76="Weeks", E76/4, E76)))</f>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="J76" s="2" t="s">
@@ -8549,7 +8800,7 @@
         <v>52</v>
       </c>
       <c r="I77" s="3">
-        <f>IF(G77="Days", E77/30, IF(G77="Years", E77*12, IF(G77="Weeks", E77/4, E77)))</f>
+        <f t="shared" si="2"/>
         <v>73.199999999999989</v>
       </c>
       <c r="J77" t="s">
@@ -8586,7 +8837,7 @@
         <v>133</v>
       </c>
       <c r="I78" s="3">
-        <f>IF(G78="Days", E78/30, IF(G78="Years", E78*12, IF(G78="Weeks", E78/4, E78)))</f>
+        <f t="shared" si="2"/>
         <v>75.599999999999994</v>
       </c>
       <c r="J78" t="s">
@@ -8623,7 +8874,7 @@
         <v>38</v>
       </c>
       <c r="I79" s="3">
-        <f>IF(G79="Days", E79/30, IF(G79="Years", E79*12, IF(G79="Weeks", E79/4, E79)))</f>
+        <f t="shared" si="2"/>
         <v>76.800000000000011</v>
       </c>
       <c r="J79" t="s">
@@ -8657,7 +8908,7 @@
         <v>33</v>
       </c>
       <c r="I80" s="3">
-        <f>IF(G80="Days", E80/30, IF(G80="Years", E80*12, IF(G80="Weeks", E80/4, E80)))</f>
+        <f t="shared" si="2"/>
         <v>77.52</v>
       </c>
       <c r="J80" t="s">
@@ -8694,7 +8945,7 @@
         <v>198</v>
       </c>
       <c r="I81" s="3">
-        <f>IF(G81="Days", E81/30, IF(G81="Years", E81*12, IF(G81="Weeks", E81/4, E81)))</f>
+        <f t="shared" si="2"/>
         <v>80.400000000000006</v>
       </c>
       <c r="J81" s="2" t="s">
@@ -8731,7 +8982,7 @@
         <v>75</v>
       </c>
       <c r="I82" s="3">
-        <f>IF(G82="Days", E82/30, IF(G82="Years", E82*12, IF(G82="Weeks", E82/4, E82)))</f>
+        <f t="shared" si="2"/>
         <v>80.400000000000006</v>
       </c>
       <c r="J82" t="s">
@@ -8768,7 +9019,7 @@
         <v>291</v>
       </c>
       <c r="I83" s="3">
-        <f>IF(G83="Days", E83/30, IF(G83="Years", E83*12, IF(G83="Weeks", E83/4, E83)))</f>
+        <f t="shared" si="2"/>
         <v>86.4</v>
       </c>
       <c r="J83" s="2" t="s">
@@ -8805,7 +9056,7 @@
         <v>265</v>
       </c>
       <c r="I84" s="3">
-        <f>IF(G84="Days", E84/30, IF(G84="Years", E84*12, IF(G84="Weeks", E84/4, E84)))</f>
+        <f t="shared" si="2"/>
         <v>87</v>
       </c>
       <c r="J84" t="s">
@@ -8842,7 +9093,7 @@
         <v>78</v>
       </c>
       <c r="I85" s="3">
-        <f>IF(G85="Days", E85/30, IF(G85="Years", E85*12, IF(G85="Weeks", E85/4, E85)))</f>
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="J85" t="s">
@@ -8879,7 +9130,7 @@
         <v>305</v>
       </c>
       <c r="I86" s="3">
-        <f>IF(G86="Days", E86/30, IF(G86="Years", E86*12, IF(G86="Weeks", E86/4, E86)))</f>
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="J86" s="2" t="s">
@@ -8916,7 +9167,7 @@
         <v>67</v>
       </c>
       <c r="I87" s="3">
-        <f>IF(G87="Days", E87/30, IF(G87="Years", E87*12, IF(G87="Weeks", E87/4, E87)))</f>
+        <f t="shared" si="2"/>
         <v>104.39999999999999</v>
       </c>
       <c r="J87" s="2" t="s">
@@ -8953,7 +9204,7 @@
         <v>67</v>
       </c>
       <c r="I88" s="3">
-        <f>IF(G88="Days", E88/30, IF(G88="Years", E88*12, IF(G88="Weeks", E88/4, E88)))</f>
+        <f t="shared" si="2"/>
         <v>106.80000000000001</v>
       </c>
       <c r="J88" t="s">
@@ -8990,7 +9241,7 @@
         <v>201</v>
       </c>
       <c r="I89" s="3">
-        <f>IF(G89="Days", E89/30, IF(G89="Years", E89*12, IF(G89="Weeks", E89/4, E89)))</f>
+        <f t="shared" si="2"/>
         <v>128.39999999999998</v>
       </c>
       <c r="J89" s="2" t="s">
@@ -9027,7 +9278,7 @@
         <v>209</v>
       </c>
       <c r="I90" s="3">
-        <f>IF(G90="Days", E90/30, IF(G90="Years", E90*12, IF(G90="Weeks", E90/4, E90)))</f>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="J90" s="2" t="s">
@@ -9064,7 +9315,7 @@
         <v>216</v>
       </c>
       <c r="I91" s="3">
-        <f>IF(G91="Days", E91/30, IF(G91="Years", E91*12, IF(G91="Weeks", E91/4, E91)))</f>
+        <f t="shared" si="2"/>
         <v>151.19999999999999</v>
       </c>
       <c r="J91" t="s">
@@ -9098,7 +9349,7 @@
         <v>33</v>
       </c>
       <c r="I92" s="3">
-        <f>IF(G92="Days", E92/30, IF(G92="Years", E92*12, IF(G92="Weeks", E92/4, E92)))</f>
+        <f t="shared" si="2"/>
         <v>156</v>
       </c>
       <c r="J92" s="2" t="s">
@@ -9129,7 +9380,7 @@
         <v>33</v>
       </c>
       <c r="I93" s="3">
-        <f>IF(G93="Days", E93/30, IF(G93="Years", E93*12, IF(G93="Weeks", E93/4, E93)))</f>
+        <f t="shared" si="2"/>
         <v>192</v>
       </c>
       <c r="J93" s="2" t="s">
@@ -9166,7 +9417,7 @@
         <v>221</v>
       </c>
       <c r="I94" s="3">
-        <f>IF(G94="Days", E94/30, IF(G94="Years", E94*12, IF(G94="Weeks", E94/4, E94)))</f>
+        <f t="shared" si="2"/>
         <v>204</v>
       </c>
       <c r="J94" s="2" t="s">
@@ -9203,7 +9454,7 @@
         <v>247</v>
       </c>
       <c r="I95" s="3">
-        <f>IF(G95="Days", E95/30, IF(G95="Years", E95*12, IF(G95="Weeks", E95/4, E95)))</f>
+        <f t="shared" si="2"/>
         <v>308.39999999999998</v>
       </c>
       <c r="J95" s="2" t="s">
@@ -9280,10 +9531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4390062C-ACD4-4ECC-BC5D-69ADAC4C3F20}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:AH163"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9295,9 +9546,10 @@
     <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9320,7 +9572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>284</v>
       </c>
@@ -9346,8 +9598,23 @@
       <c r="G2" s="2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AC2" t="s">
+        <v>368</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>411</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -9372,8 +9639,18 @@
       <c r="G3" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="13">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <f>AE3*12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -9398,8 +9675,19 @@
       <c r="G4" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE4" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="AF4" s="13">
+        <f>-(($AD$2^(1/AE4))-1)</f>
+        <v>0.99997343860111243</v>
+      </c>
+      <c r="AH4">
+        <f>AE4*12</f>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -9424,8 +9712,19 @@
       <c r="G5" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE5" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="AF5" s="13">
+        <f>-(($AD$2^(1/AE5))-1)</f>
+        <v>0.65132155989999985</v>
+      </c>
+      <c r="AH5">
+        <f>AE5*12</f>
+        <v>1.2000000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>157</v>
       </c>
@@ -9450,8 +9749,19 @@
       <c r="G6" s="2" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE6" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="AF6" s="13">
+        <f t="shared" ref="AF5:AF68" si="0">-(($AD$2^(1/AE6))-1)</f>
+        <v>0.40950999999999982</v>
+      </c>
+      <c r="AH6">
+        <f>AE6*12</f>
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -9477,8 +9787,19 @@
       <c r="G7" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE7" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AF7" s="13">
+        <f t="shared" si="0"/>
+        <v>0.23156652857908377</v>
+      </c>
+      <c r="AH7">
+        <f>AE7*12</f>
+        <v>4.8000000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>283</v>
       </c>
@@ -9503,8 +9824,19 @@
       <c r="G8" s="2" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE8" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="AF8" s="13">
+        <f t="shared" si="0"/>
+        <v>0.16104722339245814</v>
+      </c>
+      <c r="AH8">
+        <f>AE8*12</f>
+        <v>7.1999999999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>289</v>
       </c>
@@ -9529,8 +9861,19 @@
       <c r="G9" s="2" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE9" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="AF9" s="13">
+        <f t="shared" si="0"/>
+        <v>0.12339662821723285</v>
+      </c>
+      <c r="AH9">
+        <f>AE9*12</f>
+        <v>9.6000000000000014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>275</v>
       </c>
@@ -9555,8 +9898,19 @@
       <c r="G10" s="2" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE10" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="AH10">
+        <f>AE10*12</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>224</v>
       </c>
@@ -9581,8 +9935,19 @@
       <c r="G11" s="2" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE11" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="AF11" s="13">
+        <f t="shared" si="0"/>
+        <v>6.7830248213842315E-2</v>
+      </c>
+      <c r="AH11">
+        <f>AE11*12</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>162</v>
       </c>
@@ -9607,8 +9972,19 @@
       <c r="G12" s="2" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE12" s="8">
+        <v>2</v>
+      </c>
+      <c r="AF12" s="13">
+        <f t="shared" si="0"/>
+        <v>5.1316701949486232E-2</v>
+      </c>
+      <c r="AH12">
+        <f>AE12*12</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -9633,8 +10009,19 @@
       <c r="G13" s="2" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE13" s="8">
+        <v>3</v>
+      </c>
+      <c r="AF13" s="13">
+        <f t="shared" si="0"/>
+        <v>3.4510615394370281E-2</v>
+      </c>
+      <c r="AH13">
+        <f>AE13*12</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>258</v>
       </c>
@@ -9660,8 +10047,19 @@
       <c r="G14" s="2" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE14" s="8">
+        <v>4</v>
+      </c>
+      <c r="AF14" s="13">
+        <f t="shared" si="0"/>
+        <v>2.5996253574703254E-2</v>
+      </c>
+      <c r="AH14">
+        <f>AE14*12</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -9687,8 +10085,19 @@
       <c r="G15" s="2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE15" s="8">
+        <v>5</v>
+      </c>
+      <c r="AF15" s="13">
+        <f t="shared" si="0"/>
+        <v>2.0851637639023202E-2</v>
+      </c>
+      <c r="AH15">
+        <f>AE15*12</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>254</v>
       </c>
@@ -9713,8 +10122,19 @@
       <c r="G16" s="2" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE16" s="8">
+        <v>6</v>
+      </c>
+      <c r="AF16" s="13">
+        <f t="shared" si="0"/>
+        <v>1.7406806147310161E-2</v>
+      </c>
+      <c r="AH16">
+        <f>AE16*12</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -9739,8 +10159,19 @@
       <c r="G17" s="2" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE17" s="8">
+        <v>7</v>
+      </c>
+      <c r="AF17" s="13">
+        <f t="shared" si="0"/>
+        <v>1.4938794558884472E-2</v>
+      </c>
+      <c r="AH17">
+        <f>AE17*12</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>105</v>
       </c>
@@ -9765,8 +10196,19 @@
       <c r="G18" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE18" s="8">
+        <v>8</v>
+      </c>
+      <c r="AF18" s="13">
+        <f t="shared" si="0"/>
+        <v>1.3083718633998487E-2</v>
+      </c>
+      <c r="AH18">
+        <f>AE18*12</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>180</v>
       </c>
@@ -9791,8 +10233,19 @@
       <c r="G19" s="2" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE19" s="8">
+        <v>9</v>
+      </c>
+      <c r="AF19" s="13">
+        <f t="shared" si="0"/>
+        <v>1.1638466884251741E-2</v>
+      </c>
+      <c r="AH19">
+        <f>AE19*12</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>192</v>
       </c>
@@ -9817,8 +10270,19 @@
       <c r="G20" s="2" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE20" s="8">
+        <v>10</v>
+      </c>
+      <c r="AF20" s="13">
+        <f t="shared" si="0"/>
+        <v>1.0480741793785553E-2</v>
+      </c>
+      <c r="AH20">
+        <f>AE20*12</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>303</v>
       </c>
@@ -9843,8 +10307,19 @@
       <c r="G21" s="2" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE21" s="8">
+        <v>11</v>
+      </c>
+      <c r="AF21" s="13">
+        <f t="shared" si="0"/>
+        <v>9.5325035687154891E-3</v>
+      </c>
+      <c r="AH21">
+        <f>AE21*12</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>131</v>
       </c>
@@ -9869,8 +10344,18 @@
       <c r="G22" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE22" s="8">
+        <v>12</v>
+      </c>
+      <c r="AF22" s="13">
+        <f t="shared" si="0"/>
+        <v>8.7416109546967213E-3</v>
+      </c>
+      <c r="AH22">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -9895,8 +10380,10 @@
       <c r="G23" s="2" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE23" s="8"/>
+      <c r="AF23" s="13"/>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -9921,8 +10408,10 @@
       <c r="G24" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE24" s="8"/>
+      <c r="AF24" s="13"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>235</v>
       </c>
@@ -9947,8 +10436,10 @@
       <c r="G25" s="2" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE25" s="8"/>
+      <c r="AF25" s="13"/>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>264</v>
       </c>
@@ -9973,8 +10464,10 @@
       <c r="G26" s="2" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE26" s="8"/>
+      <c r="AF26" s="13"/>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>238</v>
       </c>
@@ -10000,8 +10493,10 @@
       <c r="G27" s="2" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE27" s="8"/>
+      <c r="AF27" s="13"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>199</v>
       </c>
@@ -10026,8 +10521,10 @@
       <c r="G28" s="2" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE28" s="8"/>
+      <c r="AF28" s="13"/>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -10053,8 +10550,10 @@
       <c r="G29" s="2" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE29" s="8"/>
+      <c r="AF29" s="13"/>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -10079,8 +10578,10 @@
       <c r="G30" s="2" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE30" s="8"/>
+      <c r="AF30" s="13"/>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>288</v>
       </c>
@@ -10105,8 +10606,10 @@
       <c r="G31" s="2" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE31" s="8"/>
+      <c r="AF31" s="13"/>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>304</v>
       </c>
@@ -10131,8 +10634,10 @@
       <c r="G32" s="2" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE32" s="8"/>
+      <c r="AF32" s="13"/>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>124</v>
       </c>
@@ -10157,8 +10662,10 @@
       <c r="G33" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE33" s="8"/>
+      <c r="AF33" s="13"/>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>280</v>
       </c>
@@ -10183,8 +10690,10 @@
       <c r="G34" s="2" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE34" s="8"/>
+      <c r="AF34" s="13"/>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>186</v>
       </c>
@@ -10210,8 +10719,10 @@
       <c r="G35" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE35" s="8"/>
+      <c r="AF35" s="13"/>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>200</v>
       </c>
@@ -10236,8 +10747,10 @@
       <c r="G36" s="2" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE36" s="8"/>
+      <c r="AF36" s="13"/>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -10262,8 +10775,10 @@
       <c r="G37" s="2" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE37" s="8"/>
+      <c r="AF37" s="13"/>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>262</v>
       </c>
@@ -10288,8 +10803,10 @@
       <c r="G38" s="2" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE38" s="8"/>
+      <c r="AF38" s="13"/>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>101</v>
       </c>
@@ -10314,8 +10831,10 @@
       <c r="G39" s="2" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE39" s="8"/>
+      <c r="AF39" s="13"/>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -10340,8 +10859,10 @@
       <c r="G40" s="2" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE40" s="8"/>
+      <c r="AF40" s="13"/>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -10366,8 +10887,10 @@
       <c r="G41" s="2" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE41" s="8"/>
+      <c r="AF41" s="13"/>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>137</v>
       </c>
@@ -10392,8 +10915,10 @@
       <c r="G42" s="2" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE42" s="8"/>
+      <c r="AF42" s="13"/>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -10418,8 +10943,10 @@
       <c r="G43" s="2" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE43" s="8"/>
+      <c r="AF43" s="13"/>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>242</v>
       </c>
@@ -10444,8 +10971,10 @@
       <c r="G44" s="2" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE44" s="8"/>
+      <c r="AF44" s="13"/>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>227</v>
       </c>
@@ -10470,8 +10999,10 @@
       <c r="G45" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE45" s="8"/>
+      <c r="AF45" s="13"/>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>143</v>
       </c>
@@ -10496,8 +11027,10 @@
       <c r="G46" s="2" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE46" s="8"/>
+      <c r="AF46" s="13"/>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>271</v>
       </c>
@@ -10523,8 +11056,10 @@
       <c r="G47" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE47" s="8"/>
+      <c r="AF47" s="13"/>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>296</v>
       </c>
@@ -10549,8 +11084,10 @@
       <c r="G48" s="2" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE48" s="8"/>
+      <c r="AF48" s="13"/>
+    </row>
+    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -10575,8 +11112,10 @@
       <c r="G49" s="2" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE49" s="8"/>
+      <c r="AF49" s="13"/>
+    </row>
+    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>204</v>
       </c>
@@ -10602,8 +11141,10 @@
       <c r="G50" s="2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE50" s="8"/>
+      <c r="AF50" s="13"/>
+    </row>
+    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -10628,8 +11169,10 @@
       <c r="G51" s="2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE51" s="8"/>
+      <c r="AF51" s="13"/>
+    </row>
+    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -10654,8 +11197,10 @@
       <c r="G52" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="AE52" s="8"/>
+      <c r="AF52" s="13"/>
+    </row>
+    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -10680,6 +11225,448 @@
       <c r="G53" s="2" t="s">
         <v>336</v>
       </c>
+      <c r="AE53" s="8"/>
+      <c r="AF53" s="13"/>
+    </row>
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE54" s="8"/>
+      <c r="AF54" s="13"/>
+    </row>
+    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE55" s="8"/>
+      <c r="AF55" s="13"/>
+    </row>
+    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE56" s="8"/>
+      <c r="AF56" s="13"/>
+    </row>
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE57" s="8"/>
+      <c r="AF57" s="13"/>
+    </row>
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE58" s="8"/>
+      <c r="AF58" s="13"/>
+    </row>
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE59" s="8"/>
+      <c r="AF59" s="13"/>
+    </row>
+    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE60" s="8"/>
+      <c r="AF60" s="13"/>
+    </row>
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE61" s="8"/>
+      <c r="AF61" s="13"/>
+    </row>
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE62" s="8"/>
+      <c r="AF62" s="13"/>
+    </row>
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE63" s="8"/>
+      <c r="AF63" s="13"/>
+    </row>
+    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE64" s="8"/>
+      <c r="AF64" s="13"/>
+    </row>
+    <row r="65" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE65" s="8"/>
+      <c r="AF65" s="13"/>
+    </row>
+    <row r="66" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE66" s="8"/>
+      <c r="AF66" s="13"/>
+    </row>
+    <row r="67" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE67" s="8"/>
+      <c r="AF67" s="13"/>
+    </row>
+    <row r="68" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE68" s="8"/>
+      <c r="AF68" s="13"/>
+    </row>
+    <row r="69" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE69" s="8"/>
+      <c r="AF69" s="13"/>
+    </row>
+    <row r="70" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE70" s="8"/>
+      <c r="AF70" s="13"/>
+    </row>
+    <row r="71" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE71" s="8"/>
+      <c r="AF71" s="13"/>
+    </row>
+    <row r="72" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE72" s="8"/>
+      <c r="AF72" s="13"/>
+    </row>
+    <row r="73" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE73" s="8"/>
+      <c r="AF73" s="13"/>
+    </row>
+    <row r="74" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE74" s="8"/>
+      <c r="AF74" s="13"/>
+    </row>
+    <row r="75" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE75" s="8"/>
+      <c r="AF75" s="13"/>
+    </row>
+    <row r="76" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE76" s="8"/>
+      <c r="AF76" s="13"/>
+    </row>
+    <row r="77" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE77" s="8"/>
+      <c r="AF77" s="13"/>
+    </row>
+    <row r="78" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE78" s="8"/>
+      <c r="AF78" s="13"/>
+    </row>
+    <row r="79" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE79" s="8"/>
+      <c r="AF79" s="13"/>
+    </row>
+    <row r="80" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE80" s="8"/>
+      <c r="AF80" s="13"/>
+    </row>
+    <row r="81" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE81" s="8"/>
+      <c r="AF81" s="13"/>
+    </row>
+    <row r="82" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE82" s="8"/>
+      <c r="AF82" s="13"/>
+    </row>
+    <row r="83" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE83" s="8"/>
+      <c r="AF83" s="13"/>
+    </row>
+    <row r="84" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE84" s="8"/>
+      <c r="AF84" s="13"/>
+    </row>
+    <row r="85" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE85" s="8"/>
+      <c r="AF85" s="13"/>
+    </row>
+    <row r="86" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE86" s="8"/>
+      <c r="AF86" s="13"/>
+    </row>
+    <row r="87" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE87" s="8"/>
+      <c r="AF87" s="13"/>
+    </row>
+    <row r="88" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE88" s="8"/>
+      <c r="AF88" s="13"/>
+    </row>
+    <row r="89" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE89" s="8"/>
+      <c r="AF89" s="13"/>
+    </row>
+    <row r="90" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE90" s="8"/>
+      <c r="AF90" s="13"/>
+    </row>
+    <row r="91" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE91" s="8"/>
+      <c r="AF91" s="13"/>
+    </row>
+    <row r="92" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE92" s="8"/>
+      <c r="AF92" s="13"/>
+    </row>
+    <row r="93" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE93" s="8"/>
+      <c r="AF93" s="13"/>
+    </row>
+    <row r="94" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE94" s="8"/>
+      <c r="AF94" s="13"/>
+    </row>
+    <row r="95" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE95" s="8"/>
+      <c r="AF95" s="13"/>
+    </row>
+    <row r="96" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE96" s="8"/>
+      <c r="AF96" s="13"/>
+    </row>
+    <row r="97" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE97" s="8"/>
+      <c r="AF97" s="13"/>
+    </row>
+    <row r="98" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE98" s="8"/>
+      <c r="AF98" s="13"/>
+    </row>
+    <row r="99" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE99" s="8"/>
+      <c r="AF99" s="13"/>
+    </row>
+    <row r="100" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE100" s="8"/>
+      <c r="AF100" s="13"/>
+    </row>
+    <row r="101" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE101" s="8"/>
+      <c r="AF101" s="13"/>
+    </row>
+    <row r="102" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE102" s="8"/>
+      <c r="AF102" s="13"/>
+    </row>
+    <row r="103" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE103" s="8"/>
+      <c r="AF103" s="13"/>
+    </row>
+    <row r="104" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE104" s="8"/>
+      <c r="AF104" s="13"/>
+    </row>
+    <row r="105" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE105" s="8"/>
+      <c r="AF105" s="13"/>
+    </row>
+    <row r="106" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE106" s="8"/>
+      <c r="AF106" s="13"/>
+    </row>
+    <row r="107" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE107" s="8"/>
+      <c r="AF107" s="13"/>
+    </row>
+    <row r="108" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE108" s="8"/>
+      <c r="AF108" s="13"/>
+    </row>
+    <row r="109" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE109" s="8"/>
+      <c r="AF109" s="13"/>
+    </row>
+    <row r="110" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE110" s="8"/>
+      <c r="AF110" s="13"/>
+    </row>
+    <row r="111" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE111" s="8"/>
+      <c r="AF111" s="13"/>
+    </row>
+    <row r="112" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE112" s="8"/>
+      <c r="AF112" s="13"/>
+    </row>
+    <row r="113" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE113" s="8"/>
+      <c r="AF113" s="13"/>
+    </row>
+    <row r="114" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE114" s="8"/>
+      <c r="AF114" s="13"/>
+    </row>
+    <row r="115" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE115" s="8"/>
+      <c r="AF115" s="13"/>
+    </row>
+    <row r="116" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE116" s="8"/>
+      <c r="AF116" s="13"/>
+    </row>
+    <row r="117" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE117" s="8"/>
+      <c r="AF117" s="13"/>
+    </row>
+    <row r="118" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE118" s="8"/>
+      <c r="AF118" s="13"/>
+    </row>
+    <row r="119" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE119" s="8"/>
+      <c r="AF119" s="13"/>
+    </row>
+    <row r="120" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE120" s="8"/>
+      <c r="AF120" s="13"/>
+    </row>
+    <row r="121" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE121" s="8"/>
+      <c r="AF121" s="13"/>
+    </row>
+    <row r="122" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE122" s="8"/>
+      <c r="AF122" s="13"/>
+    </row>
+    <row r="123" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE123" s="8"/>
+      <c r="AF123" s="13"/>
+    </row>
+    <row r="124" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE124" s="8"/>
+      <c r="AF124" s="13"/>
+    </row>
+    <row r="125" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE125" s="8"/>
+      <c r="AF125" s="13"/>
+    </row>
+    <row r="126" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE126" s="8"/>
+      <c r="AF126" s="13"/>
+    </row>
+    <row r="127" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE127" s="8"/>
+      <c r="AF127" s="13"/>
+    </row>
+    <row r="128" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE128" s="8"/>
+      <c r="AF128" s="13"/>
+    </row>
+    <row r="129" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE129" s="8"/>
+      <c r="AF129" s="13"/>
+    </row>
+    <row r="130" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE130" s="8"/>
+      <c r="AF130" s="13"/>
+    </row>
+    <row r="131" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE131" s="8"/>
+      <c r="AF131" s="13"/>
+    </row>
+    <row r="132" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE132" s="8"/>
+      <c r="AF132" s="13"/>
+    </row>
+    <row r="133" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE133" s="8"/>
+      <c r="AF133" s="13"/>
+    </row>
+    <row r="134" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE134" s="8"/>
+      <c r="AF134" s="13"/>
+    </row>
+    <row r="135" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE135" s="8"/>
+      <c r="AF135" s="13"/>
+    </row>
+    <row r="136" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE136" s="8"/>
+      <c r="AF136" s="13"/>
+    </row>
+    <row r="137" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE137" s="8"/>
+      <c r="AF137" s="13"/>
+    </row>
+    <row r="138" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE138" s="8"/>
+      <c r="AF138" s="13"/>
+    </row>
+    <row r="139" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE139" s="8"/>
+      <c r="AF139" s="13"/>
+    </row>
+    <row r="140" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE140" s="8"/>
+      <c r="AF140" s="13"/>
+    </row>
+    <row r="141" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE141" s="8"/>
+      <c r="AF141" s="13"/>
+    </row>
+    <row r="142" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE142" s="8"/>
+      <c r="AF142" s="13"/>
+    </row>
+    <row r="143" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE143" s="8"/>
+      <c r="AF143" s="13"/>
+    </row>
+    <row r="144" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE144" s="8"/>
+      <c r="AF144" s="13"/>
+    </row>
+    <row r="145" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE145" s="8"/>
+      <c r="AF145" s="13"/>
+    </row>
+    <row r="146" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE146" s="8"/>
+      <c r="AF146" s="13"/>
+    </row>
+    <row r="147" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE147" s="8"/>
+      <c r="AF147" s="13"/>
+    </row>
+    <row r="148" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE148" s="8"/>
+      <c r="AF148" s="13"/>
+    </row>
+    <row r="149" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE149" s="8"/>
+      <c r="AF149" s="13"/>
+    </row>
+    <row r="150" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE150" s="8"/>
+      <c r="AF150" s="13"/>
+    </row>
+    <row r="151" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE151" s="8"/>
+      <c r="AF151" s="13"/>
+    </row>
+    <row r="152" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE152" s="8"/>
+      <c r="AF152" s="13"/>
+    </row>
+    <row r="153" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE153" s="8"/>
+      <c r="AF153" s="13"/>
+    </row>
+    <row r="154" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE154" s="8"/>
+      <c r="AF154" s="13"/>
+    </row>
+    <row r="155" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE155" s="8"/>
+      <c r="AF155" s="13"/>
+    </row>
+    <row r="156" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE156" s="8"/>
+      <c r="AF156" s="13"/>
+    </row>
+    <row r="157" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE157" s="8"/>
+      <c r="AF157" s="13"/>
+    </row>
+    <row r="158" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE158" s="8"/>
+      <c r="AF158" s="13"/>
+    </row>
+    <row r="159" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE159" s="8"/>
+      <c r="AF159" s="13"/>
+    </row>
+    <row r="160" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE160" s="8"/>
+      <c r="AF160" s="13"/>
+    </row>
+    <row r="161" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE161" s="8"/>
+      <c r="AF161" s="13"/>
+    </row>
+    <row r="162" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE162" s="8"/>
+      <c r="AF162" s="13"/>
+    </row>
+    <row r="163" spans="31:32" x14ac:dyDescent="0.25">
+      <c r="AE163" s="8"/>
+      <c r="AF163" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -10745,7 +11732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1F13E5-5D80-43CB-BF4E-6BFBE4207054}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -10791,7 +11778,7 @@
       <c r="D2" t="s">
         <v>363</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>362</v>
       </c>
     </row>
@@ -10864,7 +11851,7 @@
       <c r="D7" t="s">
         <v>390</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>389</v>
       </c>
     </row>
@@ -10949,7 +11936,7 @@
       <c r="D12" t="s">
         <v>398</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>397</v>
       </c>
     </row>
@@ -11060,10 +12047,13 @@
     <hyperlink ref="F3" r:id="rId1" xr:uid="{B420FB17-4361-45D7-B47B-0C7D07D3AADB}"/>
     <hyperlink ref="F4" r:id="rId2" xr:uid="{0F4711A9-1219-4AE6-B2AC-DB3CB1F973EF}"/>
     <hyperlink ref="F6" r:id="rId3" xr:uid="{CF967FC0-D853-4ED3-A16E-AEAEDFD5BCAD}"/>
+    <hyperlink ref="F2" r:id="rId4" xr:uid="{918CA7CB-07CE-4174-BBAE-FA3CB096D24F}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{463DF5FB-CA50-4020-8673-655B39857AF3}"/>
+    <hyperlink ref="F12" r:id="rId6" xr:uid="{53F4BCF1-461B-46C0-BB41-9B6C790FBF8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -11155,8 +12145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6809CF-5461-4978-8AC5-CA059412643D}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>